<commit_message>
Creación del test para extracción del cubo de datos
</commit_message>
<xml_diff>
--- a/tests/results_tests/Estadisticos anuales.xlsx
+++ b/tests/results_tests/Estadisticos anuales.xlsx
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17.14925987180553</v>
+        <v>3.631442785263062</v>
       </c>
     </row>
     <row r="4">
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.4670731586770757</v>
+        <v>0.5939148664474487</v>
       </c>
     </row>
     <row r="5">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>16.10502915451895</v>
+        <v>2.359014749526978</v>
       </c>
     </row>
     <row r="6">
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>16.83860867731049</v>
+        <v>3.315656900405884</v>
       </c>
     </row>
     <row r="7">
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17.19194677871148</v>
+        <v>3.535092830657959</v>
       </c>
     </row>
     <row r="8">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17.45364211399075</v>
+        <v>3.891824781894684</v>
       </c>
     </row>
     <row r="9">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>18.07740740740741</v>
+        <v>5.353085517883301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>